<commit_message>
add stu note f84488efcc8b3d5309ee1596763390c75870ee89
</commit_message>
<xml_diff>
--- a/nr-add-fr-deps/ig/StructureDefinition-tlsv-observation.xlsx
+++ b/nr-add-fr-deps/ig/StructureDefinition-tlsv-observation.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-17T15:24:35+00:00</t>
+    <t>2024-10-10T08:35:45+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1350,7 +1350,7 @@
     <t>This observation is a group observation (e.g. a battery, a panel of tests, a set of vital sign measurements) that includes the target as a member of the group.</t>
   </si>
   <si>
-    <t>When using this element, an observation will typically have either a value or a set of related resources, although both may be present in some cases.  For a discussion on the ways Observations can assembled in groups together, see [Notes](http://hl7.org/fhir/R4/observation.html#obsgrouping) below.  Note that a system may calculate results from [QuestionnaireResponse](questionnaireresponse.html)  into a final score and represent the score as an Observation.</t>
+    <t>When using this element, an observation will typically have either a value or a set of related resources, although both may be present in some cases.  For a discussion on the ways Observations can assembled in groups together, see [Notes](http://hl7.org/fhir/R4/observation.html#obsgrouping) below.  Note that a system may calculate results from [QuestionnaireResponse](http://hl7.org/fhir/R4/questionnaireresponse.html)  into a final score and represent the score as an Observation.</t>
   </si>
   <si>
     <t>Relationships established by OBX-4 usage</t>

</xml_diff>